<commit_message>
data for figure 1
</commit_message>
<xml_diff>
--- a/paper/figures/originalRuntime.xlsx
+++ b/paper/figures/originalRuntime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86152\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0B2588-D6C0-4594-919B-57806F51CAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77FF8B3-BE99-40A0-B3CD-7C8C771B027E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4905" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>benchmark</t>
   </si>
@@ -71,13 +71,29 @@
     <t>threadtest</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>Dieharder</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>canneal</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>kmeans</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>reverse_index</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.0_ "/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -119,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -168,21 +190,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -260,9 +296,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>cache-scratch</c:v>
                 </c:pt>
@@ -270,21 +306,30 @@
                   <c:v>cache-thrash</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>dedup</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>freqmine</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>swaptions</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>threadtest</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>GEOMEAN</c:v>
                 </c:pt>
               </c:strCache>
@@ -292,10 +337,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -317,7 +362,16 @@
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,9 +417,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>cache-scratch</c:v>
                 </c:pt>
@@ -373,21 +427,30 @@
                   <c:v>cache-thrash</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>dedup</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>freqmine</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>swaptions</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>threadtest</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>GEOMEAN</c:v>
                 </c:pt>
               </c:strCache>
@@ -395,33 +458,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.17</c:v>
+                  <c:v>0.10251046029999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.99833253909999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.48</c:v>
+                  <c:v>1.014217259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99</c:v>
+                  <c:v>1.275696623</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.05663851</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99570180379999995</c:v>
+                  <c:v>0.99839444399999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.03</c:v>
+                  <c:v>0.99926864940000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99173553739999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.95</c:v>
+                  <c:v>1.002766252</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96192329070000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91263228760000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,9 +538,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>cache-scratch</c:v>
                 </c:pt>
@@ -476,21 +548,30 @@
                   <c:v>cache-thrash</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>dedup</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>freqmine</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>swaptions</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>threadtest</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>GEOMEAN</c:v>
                 </c:pt>
               </c:strCache>
@@ -498,33 +579,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.16</c:v>
+                  <c:v>9.9256159920000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.99714149590000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.02</c:v>
+                  <c:v>0.96431824479999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.05</c:v>
+                  <c:v>1.0040597899999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95</c:v>
+                  <c:v>1.115731716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99126268319999999</c:v>
+                  <c:v>0.91180643719999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.74</c:v>
+                  <c:v>0.94490492439999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.052892562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.91</c:v>
+                  <c:v>0.99021932420000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77570872710000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.89183443370000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -572,8 +662,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.691985471513031E-3"/>
-                  <c:y val="0.1670818664240018"/>
+                  <c:x val="9.3115756680479391E-4"/>
+                  <c:y val="0.17463484240280472"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -581,12 +671,10 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86913D95-7C77-47A8-BF1C-CBE19D5D9477}" type="VALUE">
+                    <a:r>
                       <a:rPr lang="en-US" altLang="zh-CN"/>
-                      <a:pPr/>
-                      <a:t>[VALUE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                      <a:t>3.73</a:t>
+                    </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -599,7 +687,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -611,10 +698,22 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.293592088867371E-4"/>
-                  <c:y val="0.16858095743931034"/>
+                  <c:x val="-5.5871800084294511E-4"/>
+                  <c:y val="0.17463484240280472"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>38.26</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -623,7 +722,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000E-B4BB-44F7-BB54-02C0CEB4BC98}"/>
                 </c:ext>
@@ -680,12 +781,42 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="8"/>
               <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-56B6-4C96-9F5E-64F01C3DECDA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-DB00-4AFD-8738-C92C5F2C9AD0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -697,7 +828,9 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -746,9 +879,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>cache-scratch</c:v>
                 </c:pt>
@@ -756,21 +889,30 @@
                   <c:v>cache-thrash</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>dedup</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>freqmine</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>swaptions</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>threadtest</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>GEOMEAN</c:v>
                 </c:pt>
               </c:strCache>
@@ -778,33 +920,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.26</c:v>
+                  <c:v>3.726173873</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.96</c:v>
+                  <c:v>38.263458790000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98</c:v>
+                  <c:v>0.95089303390000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.04</c:v>
+                  <c:v>0.94666912709999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79</c:v>
+                  <c:v>1.1052992559999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.016840473</c:v>
+                  <c:v>0.86371443510000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.74</c:v>
+                  <c:v>0.78589712339999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.000826446</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.22</c:v>
+                  <c:v>1.0119541590000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3652028899999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2573198999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -900,12 +1051,54 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-73B0-4EAF-B19A-0F0BA29F4E76}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-73B0-4EAF-B19A-0F0BA29F4E76}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.2021262493826896E-5"/>
-                  <c:y val="0.17155885396544843"/>
+                  <c:x val="-1.3966542375469992E-2"/>
+                  <c:y val="3.5774289665927134E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>2.07</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -914,29 +1107,31 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-73B0-4EAF-B19A-0F0BA29F4E76}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001F-73B0-4EAF-B19A-0F0BA29F4E76}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
+                  <c16:uniqueId val="{00000006-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
               <c:delete val="1"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000018-73B0-4EAF-B19A-0F0BA29F4E76}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000019-73B0-4EAF-B19A-0F0BA29F4E76}"/>
+                  <c16:uniqueId val="{00000007-DB00-4AFD-8738-C92C5F2C9AD0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -948,7 +1143,9 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -997,9 +1194,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>cache-scratch</c:v>
                 </c:pt>
@@ -1007,21 +1204,30 @@
                   <c:v>cache-thrash</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>dedup</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>freqmine</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>swaptions</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>threadtest</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>GEOMEAN</c:v>
                 </c:pt>
               </c:strCache>
@@ -1029,33 +1235,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>0.0_ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1.9281729430000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.99666507849999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92</c:v>
+                  <c:v>0.9809512494</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.01</c:v>
+                  <c:v>0.96567632400000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.87</c:v>
+                  <c:v>1.393689986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.964205186</c:v>
+                  <c:v>0.87917257859999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78</c:v>
+                  <c:v>0.86549244270000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1462809920000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.08</c:v>
+                  <c:v>2.068761114</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.57670928290000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.056970535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1066,7 +1281,427 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieharder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5860069704264216E-4"/>
+                  <c:y val="0.17463484240280472"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>2.76</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5871800084289047E-4"/>
+                  <c:y val="0.17056980045125167"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>3.67</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.3104026300450463E-4"/>
+                  <c:y val="0.1531272495766115"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>2.42</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.2849223677584405E-2"/>
+                  <c:y val="0.17463484240280472"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>5.74</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5860069704264216E-4"/>
+                  <c:y val="0.17463484240280472"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN"/>
+                      <a:t>45.64</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>cache-scratch</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cache-thrash</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>threadtest</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>GEOMEAN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.1052998606</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0555026199999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3210565919999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7516146890000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6709623850000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89074751699999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.026206728</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4223140500000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.735131397</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.642023340000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.38646544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DB00-4AFD-8738-C92C5F2C9AD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1263,10 +1898,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.25596622391897977"/>
-          <c:y val="5.2181695212116769E-2"/>
-          <c:w val="0.48931466899970844"/>
-          <c:h val="7.8437705152584705E-2"/>
+          <c:x val="0.24645601896054006"/>
+          <c:y val="6.8441863018328872E-2"/>
+          <c:w val="0.43257524188336888"/>
+          <c:h val="6.4493330930584125E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1892,16 +2527,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2192,9 +2827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2202,9 +2839,10 @@
     <col min="3" max="3" width="13.46484375" customWidth="1"/>
     <col min="5" max="5" width="11.06640625" customWidth="1"/>
     <col min="6" max="6" width="17.06640625" customWidth="1"/>
+    <col min="7" max="7" width="12.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2223,177 +2861,279 @@
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>0.17</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3.26</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2</v>
+      <c r="C2" s="7">
+        <v>0.10251046029999999</v>
+      </c>
+      <c r="D2" s="7">
+        <v>9.9256159920000003E-2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3.726173873</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1.9281729430000001</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.1052998606</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
+        <v>0.99833253909999997</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.99714149590000001</v>
+      </c>
+      <c r="E3" s="9">
+        <v>38.263458790000001</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.99666507849999997</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1.0555026199999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>20.96</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
+      <c r="C4" s="7">
+        <v>1.014217259</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.96431824479999995</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.95089303390000002</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.9809512494</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1.3210565919999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.48</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.02</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.98</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.05</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1.04</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.01</v>
+      <c r="C5" s="7">
+        <v>1.275696623</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.0040597899999999</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.94666912709999995</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.96567632400000003</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2.7516146890000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.87</v>
+      <c r="C6" s="7">
+        <v>1.05663851</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.115731716</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.1052992559999999</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.393689986</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3.6709623850000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.99570180379999995</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.99126268319999999</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.016840473</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2.964205186</v>
+      <c r="C7" s="7">
+        <v>0.99839444399999999</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.91180643719999999</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.86371443510000001</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.87917257859999998</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.89074751699999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1.74</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.78</v>
+      <c r="C8" s="7">
+        <v>0.99926864940000004</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.94490492439999996</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.78589712339999995</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.86549244270000003</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1.026206728</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.99173553739999998</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.052892562</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.000826446</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1.1462809920000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2.4223140500000002</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1.002766252</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.99021932420000003</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.0119541590000001</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2.068761114</v>
+      </c>
+      <c r="G10" s="7">
+        <v>5.735131397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.96192329070000004</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.77570872710000005</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.3652028899999999</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.57670928290000001</v>
+      </c>
+      <c r="G11" s="7">
+        <v>45.642023340000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B13" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.91</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1.22</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1.08</v>
+      <c r="C13" s="7">
+        <v>0.91263228760000004</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.89183443370000004</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.2573198999999999</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1.056970535</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1.38646544</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="B3:G13 B2:E2 G2">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>